<commit_message>
Organized files, Write up first draft
</commit_message>
<xml_diff>
--- a/Jupyter Notebook/BTC Anlys 20180428.xlsx
+++ b/Jupyter Notebook/BTC Anlys 20180428.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bryan/Dropbox/GitHub/spring-2018-final-projects-bretbryan-wt/Jupyter Notebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bwmcs\OneDrive\Documents\GitHub\spring-2018-final-projects-bretbryan-wt\Jupyter Notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA6FCC9-BFA2-9F4D-99F9-623B225B3C3E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF490145-40E6-4AED-A204-086AA200F12C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="24500" windowHeight="14980" activeTab="1" xr2:uid="{101C3BB2-7DF7-E844-B490-965F25DA06D7}"/>
+    <workbookView xWindow="156" yWindow="456" windowWidth="24504" windowHeight="14976" activeTab="1" xr2:uid="{101C3BB2-7DF7-E844-B490-965F25DA06D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="5" r:id="rId1"/>
@@ -22,9 +22,9 @@
   <definedNames>
     <definedName name="avg_end_service_surveys" localSheetId="1">Sheet1!$A$1:$AN$90</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,8 +36,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{F7FAF25F-9FA8-8740-914D-D007642841F3}" name="avg_end_service_surveys" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/Bryan/Dropbox/GitHub/spring-2018-final-projects-bretbryan-wt/Jupyter Notebook/avg_end_service_surveys.csv">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="avg_end_service_surveys" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="/Users/Bryan/Dropbox/GitHub/spring-2018-final-projects-bretbryan-wt/Jupyter Notebook/avg_end_service_surveys.csv">
       <textFields count="77">
         <textField/>
         <textField/>
@@ -9400,7 +9400,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{10B241CD-B43F-2845-9C9D-E2E4880D11E8}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{10B241CD-B43F-2845-9C9D-E2E4880D11E8}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A11:I17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="76">
     <pivotField axis="axisCol" showAll="0">
@@ -9561,31 +9561,31 @@
     <dataField name="Average of Please rate the following:The Five Step Lesson Plan Template was useful to me2" fld="9" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="9">
-    <format dxfId="0">
+    <format dxfId="8">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="7">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="6">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="5">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
     <format dxfId="4">
       <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="3">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="2">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="7">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
@@ -9606,7 +9606,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6CE75F7F-9692-0847-965B-9AF8A1BDF299}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6CE75F7F-9692-0847-965B-9AF8A1BDF299}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:I9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="76">
     <pivotField axis="axisCol" showAll="0">
@@ -9812,7 +9812,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="avg_end_service_surveys" connectionId="1" xr16:uid="{FFCF94FD-1B91-174D-BBEB-F73DE428343F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="avg_end_service_surveys" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10118,12 +10118,12 @@
       <selection activeCell="A93" sqref="A93:D196"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="26.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="26.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -10263,7 +10263,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10382,7 +10382,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -10501,7 +10501,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -10620,7 +10620,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -10739,7 +10739,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -10858,7 +10858,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -10977,7 +10977,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -11096,7 +11096,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10</v>
       </c>
@@ -11215,7 +11215,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>13</v>
       </c>
@@ -11334,7 +11334,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>14</v>
       </c>
@@ -11453,7 +11453,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>16</v>
       </c>
@@ -11572,7 +11572,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>17</v>
       </c>
@@ -11691,7 +11691,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>18</v>
       </c>
@@ -11810,7 +11810,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>19</v>
       </c>
@@ -11929,7 +11929,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>20</v>
       </c>
@@ -12048,7 +12048,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>21</v>
       </c>
@@ -12167,7 +12167,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>22</v>
       </c>
@@ -12286,7 +12286,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>23</v>
       </c>
@@ -12405,7 +12405,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>24</v>
       </c>
@@ -12524,7 +12524,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>25</v>
       </c>
@@ -12643,7 +12643,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>26</v>
       </c>
@@ -12762,7 +12762,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>27</v>
       </c>
@@ -12881,7 +12881,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>28</v>
       </c>
@@ -13000,7 +13000,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>29</v>
       </c>
@@ -13119,7 +13119,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>30</v>
       </c>
@@ -13238,7 +13238,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>31</v>
       </c>
@@ -13357,7 +13357,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>32</v>
       </c>
@@ -13476,7 +13476,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>33</v>
       </c>
@@ -13595,7 +13595,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>34</v>
       </c>
@@ -13714,7 +13714,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>35</v>
       </c>
@@ -13833,7 +13833,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>36</v>
       </c>
@@ -13952,7 +13952,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>37</v>
       </c>
@@ -14071,7 +14071,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>38</v>
       </c>
@@ -14190,7 +14190,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>39</v>
       </c>
@@ -14309,7 +14309,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>40</v>
       </c>
@@ -14428,7 +14428,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>41</v>
       </c>
@@ -14547,7 +14547,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>42</v>
       </c>
@@ -14666,7 +14666,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>45</v>
       </c>
@@ -14785,7 +14785,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>46</v>
       </c>
@@ -14904,7 +14904,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>47</v>
       </c>
@@ -15023,7 +15023,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>48</v>
       </c>
@@ -15142,7 +15142,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>49</v>
       </c>
@@ -15261,7 +15261,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>50</v>
       </c>
@@ -15380,7 +15380,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>51</v>
       </c>
@@ -15499,7 +15499,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>52</v>
       </c>
@@ -15618,7 +15618,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>53</v>
       </c>
@@ -15737,7 +15737,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>54</v>
       </c>
@@ -15856,7 +15856,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>55</v>
       </c>
@@ -15975,7 +15975,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>56</v>
       </c>
@@ -16094,7 +16094,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>57</v>
       </c>
@@ -16213,7 +16213,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>58</v>
       </c>
@@ -16332,7 +16332,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>59</v>
       </c>
@@ -16451,7 +16451,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>60</v>
       </c>
@@ -16570,7 +16570,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="55" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>62</v>
       </c>
@@ -16689,7 +16689,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>63</v>
       </c>
@@ -16808,7 +16808,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>64</v>
       </c>
@@ -16927,7 +16927,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>65</v>
       </c>
@@ -17046,7 +17046,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="59" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>66</v>
       </c>
@@ -17165,7 +17165,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>67</v>
       </c>
@@ -17284,7 +17284,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>68</v>
       </c>
@@ -17403,7 +17403,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="62" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>70</v>
       </c>
@@ -17522,7 +17522,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>71</v>
       </c>
@@ -17641,7 +17641,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="64" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>72</v>
       </c>
@@ -17760,7 +17760,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>73</v>
       </c>
@@ -17879,7 +17879,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>74</v>
       </c>
@@ -17998,7 +17998,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>75</v>
       </c>
@@ -18117,7 +18117,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="68" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>76</v>
       </c>
@@ -18236,7 +18236,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="69" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>77</v>
       </c>
@@ -18355,7 +18355,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="70" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>78</v>
       </c>
@@ -18474,7 +18474,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="71" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>79</v>
       </c>
@@ -18593,7 +18593,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="72" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>80</v>
       </c>
@@ -18712,7 +18712,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="73" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>82</v>
       </c>
@@ -18831,7 +18831,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="74" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>83</v>
       </c>
@@ -18950,7 +18950,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="75" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>85</v>
       </c>
@@ -19069,7 +19069,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="76" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>86</v>
       </c>
@@ -19188,7 +19188,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="77" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>87</v>
       </c>
@@ -19307,7 +19307,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="78" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>88</v>
       </c>
@@ -19426,7 +19426,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="79" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>89</v>
       </c>
@@ -19545,7 +19545,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="80" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>90</v>
       </c>
@@ -19664,7 +19664,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="81" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>91</v>
       </c>
@@ -19783,7 +19783,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="82" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>92</v>
       </c>
@@ -19902,7 +19902,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="83" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>93</v>
       </c>
@@ -20021,7 +20021,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="84" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>95</v>
       </c>
@@ -20140,7 +20140,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="85" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>96</v>
       </c>
@@ -20259,7 +20259,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="86" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>97</v>
       </c>
@@ -20378,7 +20378,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="87" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>98</v>
       </c>
@@ -20497,7 +20497,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="88" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>99</v>
       </c>
@@ -20616,7 +20616,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="89" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>101</v>
       </c>
@@ -20735,7 +20735,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="90" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>102</v>
       </c>
@@ -20854,14 +20854,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="93" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A93" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA93" s="6"/>
       <c r="AB93" s="6"/>
     </row>
-    <row r="94" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A94" s="8">
         <v>-0.5</v>
       </c>
@@ -21010,7 +21010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A95" s="8">
         <v>0.5</v>
       </c>
@@ -21159,7 +21159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A96" s="8">
         <v>1.5</v>
       </c>
@@ -21308,14 +21308,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A97" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA97" s="6"/>
       <c r="AB97" s="6"/>
     </row>
-    <row r="98" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A98" s="8">
         <v>-0.5</v>
       </c>
@@ -21464,7 +21464,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="99" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A99" s="8">
         <v>0.5</v>
       </c>
@@ -21613,7 +21613,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="100" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A100" s="8">
         <v>1.5</v>
       </c>
@@ -21762,14 +21762,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="101" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A101" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA101" s="6"/>
       <c r="AB101" s="6"/>
     </row>
-    <row r="102" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A102" s="8">
         <v>-0.5</v>
       </c>
@@ -21918,7 +21918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A103" s="8">
         <v>0.5</v>
       </c>
@@ -22067,7 +22067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A104" s="8">
         <v>1.5</v>
       </c>
@@ -22216,14 +22216,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A105" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA105" s="6"/>
       <c r="AB105" s="6"/>
     </row>
-    <row r="106" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A106" s="8">
         <v>-0.5</v>
       </c>
@@ -22372,7 +22372,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="107" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A107" s="8">
         <v>0.5</v>
       </c>
@@ -22521,7 +22521,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="108" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A108" s="8">
         <v>1.5</v>
       </c>
@@ -22670,14 +22670,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="109" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A109" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA109" s="6"/>
       <c r="AB109" s="6"/>
     </row>
-    <row r="110" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A110" s="8">
         <v>-0.5</v>
       </c>
@@ -22826,7 +22826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A111" s="8">
         <v>0.5</v>
       </c>
@@ -22975,7 +22975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A112" s="8">
         <v>1.5</v>
       </c>
@@ -23124,14 +23124,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A113" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA113" s="6"/>
       <c r="AB113" s="6"/>
     </row>
-    <row r="114" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A114" s="8">
         <v>-0.5</v>
       </c>
@@ -23280,7 +23280,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="115" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A115" s="8">
         <v>0.5</v>
       </c>
@@ -23429,7 +23429,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="116" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A116" s="8">
         <v>1.5</v>
       </c>
@@ -23578,14 +23578,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="117" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A117" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA117" s="6"/>
       <c r="AB117" s="6"/>
     </row>
-    <row r="118" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A118" s="8">
         <v>-0.5</v>
       </c>
@@ -23734,7 +23734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A119" s="8">
         <v>0.5</v>
       </c>
@@ -23883,7 +23883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A120" s="8">
         <v>1.5</v>
       </c>
@@ -24032,14 +24032,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A121" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA121" s="6"/>
       <c r="AB121" s="6"/>
     </row>
-    <row r="122" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A122" s="8">
         <v>-0.5</v>
       </c>
@@ -24188,7 +24188,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="123" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A123" s="8">
         <v>0.5</v>
       </c>
@@ -24337,7 +24337,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="124" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A124" s="8">
         <v>1.5</v>
       </c>
@@ -24486,7 +24486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A125" s="8">
         <v>-1.5</v>
       </c>
@@ -24635,7 +24635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A126" s="8">
         <v>-0.5</v>
       </c>
@@ -24784,7 +24784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A127" s="8">
         <v>0.5</v>
       </c>
@@ -24933,7 +24933,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="128" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A128" s="8">
         <v>1.5</v>
       </c>
@@ -25082,7 +25082,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="129" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A129" s="8">
         <v>-1.5</v>
       </c>
@@ -25231,7 +25231,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="130" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A130" s="8">
         <v>-0.5</v>
       </c>
@@ -25380,7 +25380,7 @@
         <v>-0.66666666666666663</v>
       </c>
     </row>
-    <row r="131" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A131" s="8">
         <v>0.5</v>
       </c>
@@ -25529,7 +25529,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="132" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A132" s="8">
         <v>1.5</v>
       </c>
@@ -25678,7 +25678,7 @@
         <v>0.68181818181818177</v>
       </c>
     </row>
-    <row r="133" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A133" s="8">
         <v>-1.5</v>
       </c>
@@ -25827,7 +25827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A134" s="8">
         <v>-0.5</v>
       </c>
@@ -25976,7 +25976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A135" s="8">
         <v>0.5</v>
       </c>
@@ -26125,7 +26125,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A136" s="8">
         <v>1.5</v>
       </c>
@@ -26274,7 +26274,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="137" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A137" s="8">
         <v>-1.5</v>
       </c>
@@ -26423,7 +26423,7 @@
         <v>-0.7</v>
       </c>
     </row>
-    <row r="138" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A138" s="8">
         <v>-0.5</v>
       </c>
@@ -26572,7 +26572,7 @@
         <v>-0.6</v>
       </c>
     </row>
-    <row r="139" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A139" s="8">
         <v>0.5</v>
       </c>
@@ -26721,7 +26721,7 @@
         <v>0.23333333333333334</v>
       </c>
     </row>
-    <row r="140" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A140" s="8">
         <v>1.5</v>
       </c>
@@ -26870,14 +26870,14 @@
         <v>0.88461538461538458</v>
       </c>
     </row>
-    <row r="141" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A141" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA141" s="6"/>
       <c r="AB141" s="6"/>
     </row>
-    <row r="142" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A142" s="8">
         <v>-0.5</v>
       </c>
@@ -27026,7 +27026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A143" s="8">
         <v>0.5</v>
       </c>
@@ -27175,7 +27175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="144" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A144" s="8">
         <v>1.5</v>
       </c>
@@ -27324,14 +27324,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A145" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA145" s="6"/>
       <c r="AB145" s="6"/>
     </row>
-    <row r="146" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A146" s="8">
         <v>-0.5</v>
       </c>
@@ -27480,7 +27480,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="147" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A147" s="8">
         <v>0.5</v>
       </c>
@@ -27629,7 +27629,7 @@
         <v>-0.27777777777777779</v>
       </c>
     </row>
-    <row r="148" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A148" s="8">
         <v>1.5</v>
       </c>
@@ -27778,21 +27778,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="149" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A149" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA149" s="6"/>
       <c r="AB149" s="6"/>
     </row>
-    <row r="150" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A150" s="8">
         <v>-0.5</v>
       </c>
       <c r="AA150" s="6"/>
       <c r="AB150" s="6"/>
     </row>
-    <row r="151" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A151" s="8">
         <v>0.5</v>
       </c>
@@ -27941,7 +27941,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A152" s="8">
         <v>1.5</v>
       </c>
@@ -28090,21 +28090,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A153" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA153" s="6"/>
       <c r="AB153" s="6"/>
     </row>
-    <row r="154" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A154" s="8">
         <v>-0.5</v>
       </c>
       <c r="AA154" s="6"/>
       <c r="AB154" s="6"/>
     </row>
-    <row r="155" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A155" s="8">
         <v>0.5</v>
       </c>
@@ -28253,7 +28253,7 @@
         <v>-0.31818181818181818</v>
       </c>
     </row>
-    <row r="156" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A156" s="8">
         <v>1.5</v>
       </c>
@@ -28402,21 +28402,21 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="157" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A157" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA157" s="6"/>
       <c r="AB157" s="6"/>
     </row>
-    <row r="158" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A158" s="8">
         <v>-0.5</v>
       </c>
       <c r="AA158" s="6"/>
       <c r="AB158" s="6"/>
     </row>
-    <row r="159" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A159" s="8">
         <v>0.5</v>
       </c>
@@ -28565,7 +28565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A160" s="8">
         <v>1.5</v>
       </c>
@@ -28714,21 +28714,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A161" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA161" s="6"/>
       <c r="AB161" s="6"/>
     </row>
-    <row r="162" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A162" s="8">
         <v>-0.5</v>
       </c>
       <c r="AA162" s="6"/>
       <c r="AB162" s="6"/>
     </row>
-    <row r="163" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A163" s="8">
         <v>0.5</v>
       </c>
@@ -28877,7 +28877,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="164" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A164" s="8">
         <v>1.5</v>
       </c>
@@ -29026,21 +29026,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="165" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A165" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA165" s="6"/>
       <c r="AB165" s="6"/>
     </row>
-    <row r="166" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A166" s="8">
         <v>-0.5</v>
       </c>
       <c r="AA166" s="6"/>
       <c r="AB166" s="6"/>
     </row>
-    <row r="167" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A167" s="8">
         <v>0.5</v>
       </c>
@@ -29189,7 +29189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A168" s="8">
         <v>1.5</v>
       </c>
@@ -29338,21 +29338,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A169" s="8">
         <v>-1.5</v>
       </c>
       <c r="AA169" s="6"/>
       <c r="AB169" s="6"/>
     </row>
-    <row r="170" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A170" s="8">
         <v>-0.5</v>
       </c>
       <c r="AA170" s="6"/>
       <c r="AB170" s="6"/>
     </row>
-    <row r="171" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A171" s="8">
         <v>0.5</v>
       </c>
@@ -29501,7 +29501,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="172" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A172" s="8">
         <v>1.5</v>
       </c>
@@ -29650,7 +29650,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="173" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B173" t="s">
         <v>156</v>
       </c>
@@ -29664,7 +29664,7 @@
       <c r="AA173" s="6"/>
       <c r="AB173" s="6"/>
     </row>
-    <row r="174" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B174" t="s">
         <v>156</v>
       </c>
@@ -29673,7 +29673,7 @@
       </c>
       <c r="D174" s="7"/>
     </row>
-    <row r="175" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B175" t="s">
         <v>156</v>
       </c>
@@ -29682,7 +29682,7 @@
       </c>
       <c r="D175" s="7"/>
     </row>
-    <row r="176" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B176" t="s">
         <v>156</v>
       </c>
@@ -29691,7 +29691,7 @@
       </c>
       <c r="D176" s="7"/>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B177" t="s">
         <v>156</v>
       </c>
@@ -29700,7 +29700,7 @@
       </c>
       <c r="D177" s="7"/>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B178" t="s">
         <v>156</v>
       </c>
@@ -29712,7 +29712,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B179" t="s">
         <v>156</v>
       </c>
@@ -29724,7 +29724,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B180" t="s">
         <v>156</v>
       </c>
@@ -29733,7 +29733,7 @@
       </c>
       <c r="D180" s="7"/>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B181" t="s">
         <v>156</v>
       </c>
@@ -29742,7 +29742,7 @@
       </c>
       <c r="D181" s="7"/>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B182" t="s">
         <v>156</v>
       </c>
@@ -29751,7 +29751,7 @@
       </c>
       <c r="D182" s="7"/>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B183" t="s">
         <v>156</v>
       </c>
@@ -29763,7 +29763,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B184" t="s">
         <v>156</v>
       </c>
@@ -29772,7 +29772,7 @@
       </c>
       <c r="D184" s="7"/>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B185" t="s">
         <v>156</v>
       </c>
@@ -29781,7 +29781,7 @@
       </c>
       <c r="D185" s="7"/>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B186" t="s">
         <v>156</v>
       </c>
@@ -29790,7 +29790,7 @@
       </c>
       <c r="D186" s="7"/>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B187" t="s">
         <v>156</v>
       </c>
@@ -29799,7 +29799,7 @@
       </c>
       <c r="D187" s="7"/>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B188" t="s">
         <v>156</v>
       </c>
@@ -29811,7 +29811,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B189" t="s">
         <v>156</v>
       </c>
@@ -29823,7 +29823,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B190" t="s">
         <v>156</v>
       </c>
@@ -29832,7 +29832,7 @@
       </c>
       <c r="D190" s="7"/>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B191" t="s">
         <v>156</v>
       </c>
@@ -29841,7 +29841,7 @@
       </c>
       <c r="D191" s="7"/>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B192" t="s">
         <v>156</v>
       </c>
@@ -29850,7 +29850,7 @@
       </c>
       <c r="D192" s="7"/>
     </row>
-    <row r="195" spans="3:40" x14ac:dyDescent="0.2">
+    <row r="195" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C195" t="s">
         <v>177</v>
       </c>
@@ -29999,7 +29999,7 @@
         <v>0.52641017794903955</v>
       </c>
     </row>
-    <row r="196" spans="3:40" x14ac:dyDescent="0.2">
+    <row r="196" spans="3:40" x14ac:dyDescent="0.3">
       <c r="C196" t="s">
         <v>178</v>
       </c>
@@ -30171,12 +30171,12 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="63" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -30187,7 +30187,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -30199,7 +30199,7 @@
         <v>_I_would_describe_myself_as_Resourceful</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -30207,7 +30207,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -30215,7 +30215,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -30223,7 +30223,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -30231,7 +30231,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -30239,7 +30239,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -30254,7 +30254,7 @@
         <v>Q01_PLCs_were_useful_to_me</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -30271,7 +30271,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -30288,7 +30288,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -30305,7 +30305,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -30322,7 +30322,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -30339,7 +30339,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -30356,7 +30356,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -30373,7 +30373,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -30390,7 +30390,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -30407,7 +30407,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -30424,7 +30424,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -30441,7 +30441,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -30458,7 +30458,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -30475,7 +30475,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -30492,7 +30492,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -30509,7 +30509,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -30526,7 +30526,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -30543,7 +30543,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -30563,7 +30563,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -30583,7 +30583,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -30600,7 +30600,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -30617,7 +30617,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -30634,7 +30634,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -30651,7 +30651,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -30668,7 +30668,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -30685,7 +30685,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -30702,7 +30702,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -30719,7 +30719,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -30736,7 +30736,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -30753,7 +30753,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -30770,7 +30770,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -30794,9 +30794,9 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>94</v>
       </c>
@@ -30816,7 +30816,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="F9" t="s">
         <v>132</v>
       </c>
@@ -30824,12 +30824,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="I10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
         <v>134</v>
       </c>
@@ -30846,7 +30846,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
         <v>82</v>
       </c>
@@ -30866,7 +30866,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
         <v>80</v>
       </c>
@@ -30887,7 +30887,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
         <v>76</v>
       </c>
@@ -30908,7 +30908,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
         <v>81</v>
       </c>
@@ -30929,7 +30929,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:77" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
         <v>77</v>
       </c>
@@ -30950,17 +30950,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:77" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:77" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:77" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -31190,7 +31190,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4</v>
       </c>
@@ -31423,7 +31423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -31656,7 +31656,7 @@
         <v>0.23255813953500001</v>
       </c>
     </row>
-    <row r="25" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>7</v>
       </c>
@@ -31889,7 +31889,7 @@
         <v>0.23255813953500001</v>
       </c>
     </row>
-    <row r="26" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>8</v>
       </c>
@@ -32122,7 +32122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10</v>
       </c>
@@ -32371,25 +32371,25 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.296875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" style="2"/>
+    <col min="3" max="5" width="11.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.296875" style="2"/>
     <col min="11" max="17" width="16.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="17.33203125" style="2"/>
+    <col min="18" max="16384" width="17.296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1"/>
       <c r="B1"/>
     </row>
-    <row r="3" spans="1:17" ht="128" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>138</v>
       </c>
@@ -32405,7 +32405,7 @@
       <c r="P3"/>
       <c r="Q3"/>
     </row>
-    <row r="4" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>137</v>
       </c>
@@ -32442,7 +32442,7 @@
       <c r="P4"/>
       <c r="Q4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>-1.5</v>
       </c>
@@ -32467,7 +32467,7 @@
       <c r="P5"/>
       <c r="Q5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>-0.5</v>
       </c>
@@ -32498,7 +32498,7 @@
       <c r="P6"/>
       <c r="Q6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>0.5</v>
       </c>
@@ -32535,7 +32535,7 @@
       <c r="P7"/>
       <c r="Q7"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>1.5</v>
       </c>
@@ -32572,7 +32572,7 @@
       <c r="P8"/>
       <c r="Q8"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>136</v>
       </c>
@@ -32609,7 +32609,7 @@
       <c r="P9"/>
       <c r="Q9"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -32628,7 +32628,7 @@
       <c r="P10"/>
       <c r="Q10"/>
     </row>
-    <row r="11" spans="1:17" ht="128" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>139</v>
       </c>
@@ -32644,7 +32644,7 @@
       <c r="P11"/>
       <c r="Q11"/>
     </row>
-    <row r="12" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>137</v>
       </c>
@@ -32681,7 +32681,7 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>-1.5</v>
       </c>
@@ -32698,7 +32698,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>-0.5</v>
       </c>
@@ -32721,7 +32721,7 @@
         <v>-0.26190476190476192</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>0.5</v>
       </c>
@@ -32750,7 +32750,7 @@
         <v>0.29268292682926828</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>1.5</v>
       </c>
@@ -32779,7 +32779,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>136</v>
       </c>

</xml_diff>